<commit_message>
forgot what i edited, anyway, those board sent for manufactory
</commit_message>
<xml_diff>
--- a/PCB/Project Outputs for 3DMouse/3DMouse.xlsx
+++ b/PCB/Project Outputs for 3DMouse/3DMouse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14625"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="10290"/>
   </bookViews>
   <sheets>
     <sheet name="3DMouse" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
   <si>
     <t>Comment</t>
   </si>
@@ -67,7 +67,7 @@
     <t>Header, 2-Pin</t>
   </si>
   <si>
-    <t>Battery, RESET, UART</t>
+    <t>Battery, NMI, Reset, UART</t>
   </si>
   <si>
     <t>HDR1X2</t>
@@ -94,13 +94,13 @@
     <t>Capacitor (Semiconductor SIM Model)</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C15</t>
+    <t>C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14</t>
   </si>
   <si>
     <t>CAPC2012N</t>
   </si>
   <si>
-    <t>.1uF, 1nF, 2.2uF, 4.7uF, 10nF, 22pF, 470pF</t>
+    <t>.1uF, 1nF, 2.2uF, 4.7uF, 22pF, 470pF</t>
   </si>
   <si>
     <t>LED2</t>
@@ -127,133 +127,139 @@
     <t>HDR2X5</t>
   </si>
   <si>
-    <t>Ferrite Bead</t>
-  </si>
-  <si>
-    <t>Ferrite</t>
+    <t>Header 3X2</t>
+  </si>
+  <si>
+    <t>Header, 3-Pin, Dual row</t>
+  </si>
+  <si>
+    <t>JTAG</t>
+  </si>
+  <si>
+    <t>HDR2X3</t>
+  </si>
+  <si>
+    <t>Mini USB</t>
+  </si>
+  <si>
+    <t>Mini-USB</t>
+  </si>
+  <si>
+    <t>MINI USB</t>
+  </si>
+  <si>
+    <t>Header 1-16</t>
+  </si>
+  <si>
+    <t>Header, 8-Pin, Dual row</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>HDR2X8</t>
+  </si>
+  <si>
+    <t>Header 8X2</t>
+  </si>
+  <si>
+    <t>Header 17-32</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Header 33-48</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Header 49-64</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>Header 5</t>
+  </si>
+  <si>
+    <t>Header, 5-Pin</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>HDR1X5</t>
+  </si>
+  <si>
+    <t>Header 4</t>
+  </si>
+  <si>
+    <t>Header, 4-Pin</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>HDR1X4</t>
+  </si>
+  <si>
+    <t>Header 8</t>
+  </si>
+  <si>
+    <t>Header, 6-Pin</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>HDR1X6</t>
+  </si>
+  <si>
+    <t>Header 6</t>
+  </si>
+  <si>
+    <t>Header 7</t>
+  </si>
+  <si>
+    <t>Header, 8-Pin</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>HDR1X8</t>
+  </si>
+  <si>
+    <t>P_OnBoard Sensor</t>
+  </si>
+  <si>
+    <t>Res3</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23</t>
   </si>
   <si>
     <t>RESC2012N</t>
   </si>
   <si>
-    <t>Header 3X2</t>
-  </si>
-  <si>
-    <t>Header, 3-Pin, Dual row</t>
-  </si>
-  <si>
-    <t>JTAG</t>
-  </si>
-  <si>
-    <t>HDR2X3</t>
-  </si>
-  <si>
-    <t>Mini USB</t>
-  </si>
-  <si>
-    <t>Mini-USB</t>
-  </si>
-  <si>
-    <t>MINI USB</t>
-  </si>
-  <si>
-    <t>Header 1-16</t>
-  </si>
-  <si>
-    <t>Header, 8-Pin, Dual row</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>HDR2X8</t>
-  </si>
-  <si>
-    <t>Header 8X2</t>
-  </si>
-  <si>
-    <t>Header 17-32</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>Header 33-48</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>Header 49-64</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>Header 5</t>
-  </si>
-  <si>
-    <t>Header, 5-Pin</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>HDR1X5</t>
-  </si>
-  <si>
-    <t>Header 4</t>
-  </si>
-  <si>
-    <t>Header, 4-Pin</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>HDR1X4</t>
-  </si>
-  <si>
-    <t>Header 8</t>
-  </si>
-  <si>
-    <t>Header, 6-Pin</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>HDR1X6</t>
-  </si>
-  <si>
-    <t>Header 6</t>
-  </si>
-  <si>
-    <t>Header 7</t>
-  </si>
-  <si>
-    <t>Header, 8-Pin</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>HDR1X8</t>
-  </si>
-  <si>
-    <t>P_OnBoard Sensor</t>
-  </si>
-  <si>
-    <t>Res3</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22</t>
-  </si>
-  <si>
-    <t>1k, 10k, 39, 80.6, 250k</t>
+    <t>1k, 10k, 39, 80.6</t>
+  </si>
+  <si>
+    <t>SW-SPDT</t>
+  </si>
+  <si>
+    <t>SPDT Subminiature Toggle Switch, Right Angle Mounting, Vertical Actuation</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>563-1102-1-ND</t>
   </si>
   <si>
     <t>74LV4051</t>
@@ -280,7 +286,7 @@
     <t>TQFP64_N - ECESHOP</t>
   </si>
   <si>
-    <t>XTAL 16Mhz</t>
+    <t>XTAL 12Mhz</t>
   </si>
   <si>
     <t>Crystal Oscillator</t>
@@ -767,7 +773,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>11</v>
@@ -813,7 +819,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>28</v>
@@ -870,13 +876,13 @@
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>37</v>
@@ -890,10 +896,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>42</v>
@@ -902,7 +908,7 @@
         <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -916,16 +922,16 @@
         <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -936,19 +942,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -959,19 +965,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -982,19 +988,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -1005,19 +1011,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -1028,19 +1034,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1051,19 +1057,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1074,19 +1080,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -1097,19 +1103,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -1120,65 +1126,65 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="F20" s="3">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F21" s="3">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="F22" s="3">
         <v>2</v>
@@ -1189,13 +1195,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>18</v>
@@ -1212,19 +1218,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
@@ -1235,19 +1241,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
@@ -1258,19 +1264,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>

</xml_diff>